<commit_message>
Branch & Bound Working
</commit_message>
<xml_diff>
--- a/TODOs.xlsx
+++ b/TODOs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799478E6-1E67-4A99-85F1-65695AF6A19B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D665F29D-0763-4931-913A-9D767DEDC08A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Thing to do</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Write Report</t>
+  </si>
+  <si>
+    <t>Report - What do you want? Special requests? I'm gonna invest</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="C1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,12 +705,14 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>